<commit_message>
More comments removed any windows dependency
</commit_message>
<xml_diff>
--- a/src/OCRProject/Output/Comparision/ProcessingResults.xlsx
+++ b/src/OCRProject/Output/Comparision/ProcessingResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Image Name</t>
   </si>
@@ -23,22 +23,10 @@
     <t xml:space="preserve">Time Taken (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">sample-image</t>
+    <t xml:space="preserve">ocr_preprocessing_input</t>
   </si>
   <si>
     <t xml:space="preserve">Grayscale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GlobalThreshold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shifted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SaturationAdjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deskewed</t>
   </si>
 </sst>
 </file>
@@ -83,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
@@ -108,51 +96,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="0">
-        <v>1.2524604</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0">
-        <v>1.0849144</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0">
-        <v>0.097008</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="0">
-        <v>0.1318487</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="0">
-        <v>4.2191572</v>
+        <v>16.1419122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added backup embedding generator
</commit_message>
<xml_diff>
--- a/src/OCRProject/Output/Comparision/ProcessingResults.xlsx
+++ b/src/OCRProject/Output/Comparision/ProcessingResults.xlsx
@@ -6,39 +6,66 @@
     <workbookView tabRatio="600"/>
   </bookViews>
   <sheets>
-    <sheet name="Processing Times" sheetId="1" r:id="rId3"/>
+    <sheet name="Processing Results" sheetId="1" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">Image Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Taken (s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">special-characters</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Time (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Memory (MB)</t>
   </si>
   <si>
     <t xml:space="preserve">Grayscale</t>
   </si>
   <si>
-    <t xml:space="preserve">GlobalThreshold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SaturationAdjusted</t>
+    <t xml:space="preserve">GlobalThreshold_80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalThreshold_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalThreshold_110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalThreshold_120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalThreshold_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalThreshold_150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaturationAdjusted_1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaturationAdjusted_0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaturationAdjusted_0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaturationAdjusted_1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaturationAdjusted_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaturationAdjusted_2.5</t>
   </si>
   <si>
     <t xml:space="preserve">Deskewed</t>
   </si>
   <si>
-    <t xml:space="preserve">Memory Usage (MB)</t>
+    <t xml:space="preserve">AdaptiveThreshold</t>
   </si>
 </sst>
 </file>
@@ -83,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
@@ -99,64 +126,170 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
+      <c r="B2" s="0">
+        <v>3487.4503</v>
       </c>
       <c r="C2" s="0">
-        <v>0.0330983</v>
-      </c>
-      <c r="D2" s="0">
-        <v>0.23</v>
+        <v>0.0174102783203125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="0">
+        <v>2030.5106</v>
       </c>
       <c r="C3" s="0">
-        <v>0.013891</v>
-      </c>
-      <c r="D3" s="0">
-        <v>-0.09</v>
+        <v>0.00153350830078125</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="0">
+        <v>1852.6646</v>
       </c>
       <c r="C4" s="0">
-        <v>0.0136268</v>
-      </c>
-      <c r="D4" s="0">
-        <v>0.18</v>
+        <v>0.001556396484375</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0">
+        <v>1883.6105</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="0">
-        <v>0.0387508</v>
-      </c>
-      <c r="D5" s="0">
-        <v>0.46</v>
+      <c r="B6" s="0">
+        <v>1855.9105</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1894.1727</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1864.0743</v>
+      </c>
+      <c r="C8" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="0">
+        <v>2414.8405</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="0">
+        <v>2499.9113</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="0">
+        <v>2333.0732</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="0">
+        <v>2304.316</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="0">
+        <v>2361.7887</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0">
+        <v>2466.5393</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0.001556396484375</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="0">
+        <v>2182.308</v>
+      </c>
+      <c r="C15" s="0">
+        <v>2.4687118530273438</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="0">
+        <v>4926.2778</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0.0014190673828125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>